<commit_message>
Feat sending zip files
</commit_message>
<xml_diff>
--- a/excel-files/image/image-url.xlsx
+++ b/excel-files/image/image-url.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geffe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C631928-91C4-4222-AB25-DFB90A1DD041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{813716F3-EA7F-4C06-8B77-6E95B1C937B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B9850FB-3DED-4EEE-9074-541AEF78CC97}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$A$431</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2235,8 +2238,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB1A4827-8481-4A28-9482-4A98454EB8C2}">
   <dimension ref="A1:B431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
-      <selection activeCell="J305" sqref="J305"/>
+    <sheetView tabSelected="1" topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="A299" sqref="A293:XFD299"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4769,6 +4772,7 @@
     <row r="430" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="431" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <autoFilter ref="A1:A431" xr:uid="{BB1A4827-8481-4A28-9482-4A98454EB8C2}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>